<commit_message>
up lại các note_DoanCuong lúc trước di chuyển vào github/home
</commit_message>
<xml_diff>
--- a/deploy/backend/example/data.xlsx
+++ b/deploy/backend/example/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/cuong_dn210141_sis_hust_edu_vn/Documents/Data Manager/XONG XÓA/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://husteduvn-my.sharepoint.com/personal/cuong_dn210141_sis_hust_edu_vn/Documents/GIT/MiniProd_ContentEngFlow_IELTSStepUpE_T102024/deploy/backend/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_690C9FCDAE3DB4E6AB6EC90AFCAE670FAE24A5A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE08523C-205E-43CE-AB78-18DAFEA346C0}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="11_690C9FCDAE3DB4E6AB6EC90AFCAE670FAE24A5A1" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8B2E838-37BB-4A8C-8A77-ECB961B60FE9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>order</t>
   </si>
@@ -133,6 +133,9 @@
   <si>
     <t>Topic: Family size and type
 Vocab: Generational family</t>
+  </si>
+  <si>
+    <t>week</t>
   </si>
   <si>
     <t>set</t>
@@ -576,222 +579,231 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="31" style="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="60.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.44140625" style="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" style="16" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" style="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31" style="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="9.109375" style="16" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="60.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="15" max="17" width="13.5546875" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" s="1" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="F1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
     </row>
-    <row r="2" spans="1:16" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="6">
-        <v>999</v>
-      </c>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:17" s="1" customFormat="1" ht="409.6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="16">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="str">
-        <f>"Topic: "&amp;D2&amp;" - "&amp;E2&amp;CHAR(10)&amp;"Given vocabulary: "&amp;F2&amp;CHAR(10)&amp;"Situation: "&amp;G2</f>
+      <c r="B2" s="6">
+        <v>3000</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="7" t="str">
+        <f>"Topic: "&amp;E2&amp;" - "&amp;F2&amp;CHAR(10)&amp;"Given vocabulary: "&amp;G2&amp;CHAR(10)&amp;"Situation: "&amp;H2</f>
         <v>Topic: talk about your family - Family size and type
 Given vocabulary: Nuclear family
 Situation: Sarah and Tom, neighbors, at a community park</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="K2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="L2" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="8"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="8"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="10" t="str">
-        <f>N2&amp;""""&amp;F2&amp;""""&amp;O2&amp;A2&amp;"/ipa.mp3"</f>
-        <v>curl -L -X POST 'http://103.253.20.13:25010/api/text-to-speech' -H 'Content-Type: application/json' -d '{"text": "Nuclear family","voice": "en-CA-ClaraNeural","speed": 1}' --output 999/ipa.mp3</v>
+      <c r="Q2" s="10" t="str">
+        <f>O2&amp;""""&amp;G2&amp;""""&amp;P2&amp;B2&amp;"/ipa.mp3"</f>
+        <v>curl -L -X POST 'http://103.253.20.13:25010/api/text-to-speech' -H 'Content-Type: application/json' -d '{"text": "Nuclear family","voice": "en-CA-ClaraNeural","speed": 1}' --output 3000/ipa.mp3</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="409.6" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="6">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:17" ht="409.6" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3" s="6">
+        <v>2000</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="7" t="str">
-        <f>"Topic: "&amp;D3&amp;" - "&amp;E3&amp;CHAR(10)&amp;"Given vocabulary: "&amp;F3&amp;CHAR(10)&amp;"Situation: "&amp;G3</f>
+      <c r="D3" s="7" t="str">
+        <f>"Topic: "&amp;E3&amp;" - "&amp;F3&amp;CHAR(10)&amp;"Given vocabulary: "&amp;G3&amp;CHAR(10)&amp;"Situation: "&amp;H3</f>
         <v>Topic: talk about your family - Family size and type
 Given vocabulary: Generational family
 Situation: Aubrey and Isaac, engineers, at a construction site</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="E3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="G3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="L3" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="8"/>
-      <c r="M3" s="9"/>
-      <c r="N3" s="11" t="s">
+      <c r="M3" s="8"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="P3" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="12" t="str">
-        <f>N3&amp;""""&amp;F3&amp;""""&amp;O3&amp;A3&amp;"/ipa.MP4"</f>
-        <v>curl -L -X POST 'http://103.253.20.13:25010/api/text-to-speech' -H 'Content-Type: application/json' -d '{"text": "Generational family","voice": "en-CA-ClaraNeural","speed": 1}' --output 2/ipa.MP4</v>
+      <c r="Q3" s="12" t="str">
+        <f>O3&amp;""""&amp;G3&amp;""""&amp;P3&amp;B3&amp;"/ipa.MP4"</f>
+        <v>curl -L -X POST 'http://103.253.20.13:25010/api/text-to-speech' -H 'Content-Type: application/json' -d '{"text": "Generational family","voice": "en-CA-ClaraNeural","speed": 1}' --output 2000/ipa.MP4</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="5"/>
+    <row r="4" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="13"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="14"/>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
       <c r="M4" s="5"/>
-      <c r="N4" s="11"/>
+      <c r="N4" s="5"/>
       <c r="O4" s="11"/>
       <c r="P4" s="11"/>
+      <c r="Q4" s="11"/>
     </row>
-    <row r="5" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="5"/>
+    <row r="5" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="13"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
-      <c r="N5" s="11"/>
+      <c r="N5" s="5"/>
       <c r="O5" s="11"/>
       <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
     </row>
-    <row r="6" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="5"/>
+    <row r="6" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="13"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
       <c r="L6" s="5"/>
       <c r="M6" s="5"/>
-      <c r="N6" s="11"/>
+      <c r="N6" s="5"/>
       <c r="O6" s="11"/>
       <c r="P6" s="11"/>
+      <c r="Q6" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>